<commit_message>
improve: ubah urutan dan bahasa header excel
</commit_message>
<xml_diff>
--- a/storage/app/templates/template-import-teacher.xlsx
+++ b/storage/app/templates/template-import-teacher.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dev\Projects\php\laravel-school\storage\app\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66C7B72A-D746-467C-986E-A9CA2CA46C24}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{941AD445-D3C4-487C-BDFC-3D9C507BD9E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="21825" windowHeight="11460" xr2:uid="{79DDDC3B-40F5-4408-A8FB-897D13C97370}"/>
+    <workbookView xWindow="9420" yWindow="2595" windowWidth="21825" windowHeight="11460" xr2:uid="{79DDDC3B-40F5-4408-A8FB-897D13C97370}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,33 +25,30 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>email</t>
-  </si>
-  <si>
-    <t>phone</t>
-  </si>
-  <si>
-    <t>address</t>
-  </si>
-  <si>
-    <t>nip</t>
-  </si>
-  <si>
-    <t>position</t>
-  </si>
-  <si>
-    <t>username*</t>
-  </si>
-  <si>
-    <t>password*</t>
-  </si>
-  <si>
-    <t>status*</t>
-  </si>
-  <si>
-    <t>full name*</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+  <si>
+    <t>Nama Lengkap*</t>
+  </si>
+  <si>
+    <t>Username*</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>NIP</t>
+  </si>
+  <si>
+    <t>Nomor Telepon</t>
+  </si>
+  <si>
+    <t>Alamat</t>
+  </si>
+  <si>
+    <t>Password*</t>
+  </si>
+  <si>
+    <t>Posisi</t>
   </si>
 </sst>
 </file>
@@ -89,7 +86,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -112,13 +109,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -437,7 +453,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79BA89CC-DE0C-4429-9338-60B9A8E2327B}">
   <dimension ref="A1:I1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G7" sqref="G7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -453,32 +471,30 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>4</v>
-      </c>
+      <c r="I1" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>